<commit_message>
Search skill by category implementation
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t xml:space="preserve">FirstName</t>
   </si>
@@ -57,9 +57,21 @@
     <t xml:space="preserve">Username</t>
   </si>
   <si>
+    <t xml:space="preserve">Current Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confirm Password</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://www.skillswap.pro/Home</t>
   </si>
   <si>
+    <t xml:space="preserve">Shilpi@01</t>
+  </si>
+  <si>
     <t xml:space="preserve">AvailableTime</t>
   </si>
   <si>
@@ -138,7 +150,7 @@
     <t xml:space="preserve">ANZTB</t>
   </si>
   <si>
-    <t xml:space="preserve">3 years as Oracle Developer and 2 years as Project Management Operations Lead</t>
+    <t xml:space="preserve">Selenium is an automation test suits. It is open source tool it can sopurt multiple language.</t>
   </si>
 </sst>
 </file>
@@ -395,10 +407,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -406,7 +418,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -417,25 +431,39 @@
         <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="http://www.skillswap.pro/Home"/>
     <hyperlink ref="B2" r:id="rId2" display="vidhyav9@gmail.com"/>
-    <hyperlink ref="C2" r:id="rId3" display="Ithika2015"/>
+    <hyperlink ref="C2" r:id="rId3" display="Shilpi@01"/>
+    <hyperlink ref="D2" r:id="rId4" display="Shilpi@01"/>
+    <hyperlink ref="E2" r:id="rId5" display="Shilpi@01"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -454,8 +482,8 @@
   </sheetPr>
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -473,90 +501,90 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>